<commit_message>
Build a new model coefficients table
Former-commit-id: 22c04f6293d35954929280a29d792eb7e54d0e1f
</commit_message>
<xml_diff>
--- a/data/DC_Parameters.xlsx
+++ b/data/DC_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbarnes/Documents/GitHub/resiliency_paper/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregmacfarlane/projects/resiliency_paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D12FDF-3ACE-DA4E-85EC-6096D667F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD61C47D-30D0-0C46-B2E6-23D6353BDD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{1E23727F-5EFC-FA4B-9B79-247A2184F293}"/>
+    <workbookView xWindow="21140" yWindow="16640" windowWidth="28040" windowHeight="17440" xr2:uid="{1E23727F-5EFC-FA4B-9B79-247A2184F293}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>HBW</t>
   </si>
   <si>
@@ -48,16 +45,19 @@
     <t>NHB</t>
   </si>
   <si>
-    <t>HH</t>
-  </si>
-  <si>
-    <t>OFF_EMP</t>
-  </si>
-  <si>
-    <t>OTH_EMP</t>
-  </si>
-  <si>
-    <t>RET_EMP</t>
+    <t>var</t>
+  </si>
+  <si>
+    <t>Households</t>
+  </si>
+  <si>
+    <t>Office Employment</t>
+  </si>
+  <si>
+    <t>Other Employment</t>
+  </si>
+  <si>
+    <t>Retail Employment</t>
   </si>
 </sst>
 </file>
@@ -424,23 +424,26 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Combine dc parameters into single file
Former-commit-id: 52d2f67a1ffc2603063fa1c4772bae473385f594
</commit_message>
<xml_diff>
--- a/data/DC_Parameters.xlsx
+++ b/data/DC_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregmacfarlane/projects/resiliency_paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD61C47D-30D0-0C46-B2E6-23D6353BDD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CA5FCC-DDB8-794B-A122-62E4CD367214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21140" yWindow="16640" windowWidth="28040" windowHeight="17440" xr2:uid="{1E23727F-5EFC-FA4B-9B79-247A2184F293}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>HBW</t>
   </si>
@@ -58,6 +58,51 @@
   </si>
   <si>
     <t>Retail Employment</t>
+  </si>
+  <si>
+    <t>-0.0801 </t>
+  </si>
+  <si>
+    <t>-0.1728 </t>
+  </si>
+  <si>
+    <t>-0.1157 </t>
+  </si>
+  <si>
+    <t>0.3151 </t>
+  </si>
+  <si>
+    <t>0.0026 </t>
+  </si>
+  <si>
+    <t>0.0034 </t>
+  </si>
+  <si>
+    <t>0.0035 </t>
+  </si>
+  <si>
+    <t>-0.0026 </t>
+  </si>
+  <si>
+    <t>-0.0000090 </t>
+  </si>
+  <si>
+    <t>-0.0000110 </t>
+  </si>
+  <si>
+    <t>-0.0000133 </t>
+  </si>
+  <si>
+    <t>0.0000055 </t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Distance^2</t>
+  </si>
+  <si>
+    <t>Distance^3</t>
   </si>
 </sst>
 </file>
@@ -99,13 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A02DF32-83E4-E14A-9038-E2CAD9855466}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,7 +480,7 @@
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -446,7 +494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -460,7 +508,7 @@
         <v>0.2077</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -474,7 +522,7 @@
         <v>0.28160000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -488,7 +536,7 @@
         <v>0.28160000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -500,6 +548,57 @@
       </c>
       <c r="D5" s="2">
         <v>5.1185999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>